<commit_message>
added DataAccess and API
</commit_message>
<xml_diff>
--- a/StatementBank/bin/Debug/net6.0/NeamtuStatement.xlsx
+++ b/StatementBank/bin/Debug/net6.0/NeamtuStatement.xlsx
@@ -471,7 +471,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="E2" s="1">
-        <x:v>45125.5933820602</x:v>
+        <x:v>45132.4698562732</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
@@ -488,7 +488,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="E3" s="1">
-        <x:v>45125.5933820949</x:v>
+        <x:v>45132.4698563079</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
@@ -505,7 +505,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E4" s="1">
-        <x:v>45125.5933820949</x:v>
+        <x:v>45132.4698563079</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -522,7 +522,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="E5" s="1">
-        <x:v>45125.5933820949</x:v>
+        <x:v>45132.4698563079</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
@@ -539,7 +539,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="E6" s="1">
-        <x:v>45125.5933820949</x:v>
+        <x:v>45132.4698563079</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
@@ -556,7 +556,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="E7" s="1">
-        <x:v>45125.5933820949</x:v>
+        <x:v>45132.4698563079</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
@@ -573,7 +573,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="E8" s="1">
-        <x:v>45125.5933820949</x:v>
+        <x:v>45132.4698563079</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>